<commit_message>
mise à jour de la base de données
</commit_message>
<xml_diff>
--- a/Suivi_projet_yasin_Akgedik.xlsx
+++ b/Suivi_projet_yasin_Akgedik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\cinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6FBCB4-2E93-48BB-9353-BC43DE411C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A12879-A047-4368-803C-72D3A274223E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CF539EC5-3BDF-4CE5-B05E-309A2D75A2C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
   <si>
     <t>Prénom NOM</t>
   </si>
@@ -117,6 +117,27 @@
   </si>
   <si>
     <t>Cards listRoles.css</t>
+  </si>
+  <si>
+    <t>GenreController.php : listGenre()</t>
+  </si>
+  <si>
+    <t>GenreController.php : infosGenre()</t>
+  </si>
+  <si>
+    <t>listGenres.php</t>
+  </si>
+  <si>
+    <t>infosGenre.php</t>
+  </si>
+  <si>
+    <t>case "listGenres"</t>
+  </si>
+  <si>
+    <t>case "infosGenres"</t>
+  </si>
+  <si>
+    <t>implanter les images (en cours)</t>
   </si>
 </sst>
 </file>
@@ -426,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,76 +476,79 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -850,7 +874,7 @@
   <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,1123 +901,1107 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="24" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="22" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="32"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="33"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="23">
         <v>45092</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="18" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="21" t="s">
+      <c r="F6" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="19"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="11"/>
+      <c r="F7" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="32"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="11"/>
+      <c r="F8" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="32"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="19"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="11"/>
+      <c r="F9" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="19"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="11"/>
+      <c r="F10" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="19"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="11"/>
+      <c r="F11" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="30"/>
       <c r="E12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="11"/>
+      <c r="F12" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="22"/>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="19"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="11"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="20"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="31"/>
       <c r="E14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="11"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="23">
         <v>45093</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="18" t="s">
+      <c r="C15" s="26"/>
+      <c r="D15" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="19"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="9"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="11"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="22"/>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="19"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="9"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="11"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="22"/>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="19"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="9"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="11"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="22"/>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="19"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="9"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="11"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="22"/>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="19"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="9"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="11"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="22"/>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="19"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="9"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="11"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="19"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="30"/>
       <c r="E22" s="9"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="11"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="20"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="8"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="11"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
+      <c r="A24" s="23">
         <v>45094</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="18" t="s">
+      <c r="C24" s="26"/>
+      <c r="D24" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="I24" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="19"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="9"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="11"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="19"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="9"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="11"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" spans="1:9" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="19"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="9"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="11"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="22"/>
     </row>
     <row r="28" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="19"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="30"/>
       <c r="E28" s="9"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="11"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="22"/>
     </row>
     <row r="29" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="19"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="9"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="11"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="22"/>
     </row>
     <row r="30" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="19"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="30"/>
       <c r="E30" s="9"/>
       <c r="F30" s="7"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="11"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="22"/>
     </row>
     <row r="31" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="19"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="9"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="11"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="20"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="8"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="11"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="22"/>
     </row>
     <row r="33" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
+      <c r="A33" s="23">
         <v>45095</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="18" t="s">
+      <c r="C33" s="26"/>
+      <c r="D33" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="21" t="s">
+      <c r="G33" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I33" s="11" t="s">
+      <c r="I33" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="19"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="9"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="11"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="22"/>
     </row>
     <row r="35" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="19"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="30"/>
       <c r="E35" s="9"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="11"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="22"/>
     </row>
     <row r="36" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="19"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="9"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="11"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="22"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="19"/>
+      <c r="A37" s="24"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="9"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="11"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="22"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="19"/>
+      <c r="A38" s="24"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="30"/>
       <c r="E38" s="9"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="11"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="22"/>
     </row>
     <row r="39" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="19"/>
+      <c r="A39" s="24"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="30"/>
       <c r="E39" s="9"/>
       <c r="F39" s="7"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="11"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="22"/>
     </row>
     <row r="40" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="19"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="30"/>
       <c r="E40" s="9"/>
       <c r="F40" s="7"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="11"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="22"/>
     </row>
     <row r="41" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="20"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="31"/>
       <c r="E41" s="8"/>
       <c r="F41" s="7"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="11"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="22"/>
     </row>
     <row r="42" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="12">
+      <c r="A42" s="23">
         <v>45096</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="18" t="s">
+      <c r="C42" s="26"/>
+      <c r="D42" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="7"/>
-      <c r="G42" s="21" t="s">
+      <c r="G42" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H42" s="10" t="s">
+      <c r="H42" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I42" s="11" t="s">
+      <c r="I42" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="19"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="30"/>
       <c r="E43" s="9"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="11"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="22"/>
     </row>
     <row r="44" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="19"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="9"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="10"/>
-      <c r="I44" s="11"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="22"/>
     </row>
     <row r="45" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="19"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="30"/>
       <c r="E45" s="9"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="11"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="22"/>
     </row>
     <row r="46" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="19"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="30"/>
       <c r="E46" s="9"/>
       <c r="F46" s="7"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="11"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="22"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="19"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="30"/>
       <c r="E47" s="9"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="10"/>
-      <c r="I47" s="11"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="22"/>
     </row>
     <row r="48" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="19"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="9"/>
       <c r="F48" s="7"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="11"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="22"/>
     </row>
     <row r="49" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="19"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="9"/>
       <c r="F49" s="7"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="10"/>
-      <c r="I49" s="11"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="22"/>
     </row>
     <row r="50" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="20"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="31"/>
       <c r="E50" s="8"/>
       <c r="F50" s="7"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="11"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="22"/>
     </row>
     <row r="51" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="12">
+      <c r="A51" s="23">
         <v>45097</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="18" t="s">
+      <c r="C51" s="26"/>
+      <c r="D51" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="7"/>
-      <c r="G51" s="21" t="s">
+      <c r="G51" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H51" s="10" t="s">
+      <c r="H51" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I51" s="11" t="s">
+      <c r="I51" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="19"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="30"/>
       <c r="E52" s="9"/>
       <c r="F52" s="7"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="10"/>
-      <c r="I52" s="11"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="22"/>
     </row>
     <row r="53" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="19"/>
+      <c r="A53" s="24"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="30"/>
       <c r="E53" s="9"/>
       <c r="F53" s="7"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="11"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="22"/>
     </row>
     <row r="54" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="19"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="30"/>
       <c r="E54" s="9"/>
       <c r="F54" s="7"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="11"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="22"/>
     </row>
     <row r="55" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="19"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="30"/>
       <c r="E55" s="9"/>
       <c r="F55" s="7"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="11"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="22"/>
     </row>
     <row r="56" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="19"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="9"/>
       <c r="F56" s="7"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="11"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="22"/>
     </row>
     <row r="57" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="19"/>
+      <c r="A57" s="24"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="30"/>
       <c r="E57" s="9"/>
       <c r="F57" s="7"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="11"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="22"/>
     </row>
     <row r="58" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="19"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="30"/>
       <c r="E58" s="9"/>
       <c r="F58" s="7"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="11"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="22"/>
     </row>
     <row r="59" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="20"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="31"/>
       <c r="E59" s="8"/>
       <c r="F59" s="7"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="10"/>
-      <c r="I59" s="11"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="22"/>
     </row>
     <row r="60" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="12">
+      <c r="A60" s="23">
         <v>45098</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="18" t="s">
+      <c r="C60" s="26"/>
+      <c r="D60" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="7"/>
-      <c r="G60" s="21" t="s">
+      <c r="G60" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H60" s="10" t="s">
+      <c r="H60" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I60" s="11" t="s">
+      <c r="I60" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="19"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="30"/>
       <c r="E61" s="9"/>
       <c r="F61" s="7"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="11"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="22"/>
     </row>
     <row r="62" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="19"/>
+      <c r="A62" s="24"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="30"/>
       <c r="E62" s="9"/>
       <c r="F62" s="7"/>
-      <c r="G62" s="21"/>
-      <c r="H62" s="10"/>
-      <c r="I62" s="11"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="22"/>
     </row>
     <row r="63" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="19"/>
+      <c r="A63" s="24"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="30"/>
       <c r="E63" s="9"/>
       <c r="F63" s="7"/>
-      <c r="G63" s="21"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="11"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="33"/>
+      <c r="I63" s="22"/>
     </row>
     <row r="64" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="19"/>
+      <c r="A64" s="24"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="30"/>
       <c r="E64" s="9"/>
       <c r="F64" s="7"/>
-      <c r="G64" s="21"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="11"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="22"/>
     </row>
     <row r="65" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="19"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="30"/>
       <c r="E65" s="9"/>
       <c r="F65" s="7"/>
-      <c r="G65" s="21"/>
-      <c r="H65" s="10"/>
-      <c r="I65" s="11"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="33"/>
+      <c r="I65" s="22"/>
     </row>
     <row r="66" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="19"/>
+      <c r="A66" s="24"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="30"/>
       <c r="E66" s="9"/>
       <c r="F66" s="7"/>
-      <c r="G66" s="21"/>
-      <c r="H66" s="10"/>
-      <c r="I66" s="11"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="22"/>
     </row>
     <row r="67" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="16"/>
-      <c r="D67" s="19"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="30"/>
       <c r="E67" s="9"/>
       <c r="F67" s="7"/>
-      <c r="G67" s="21"/>
-      <c r="H67" s="10"/>
-      <c r="I67" s="11"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="22"/>
     </row>
     <row r="68" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="17"/>
-      <c r="D68" s="20"/>
+      <c r="A68" s="25"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="31"/>
       <c r="E68" s="8"/>
       <c r="F68" s="7"/>
-      <c r="G68" s="21"/>
-      <c r="H68" s="10"/>
-      <c r="I68" s="11"/>
+      <c r="G68" s="32"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="22"/>
     </row>
     <row r="69" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="12">
+      <c r="A69" s="23">
         <v>45099</v>
       </c>
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="18" t="s">
+      <c r="C69" s="26"/>
+      <c r="D69" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="7"/>
-      <c r="G69" s="21" t="s">
+      <c r="G69" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H69" s="10" t="s">
+      <c r="H69" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I69" s="11" t="s">
+      <c r="I69" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
-      <c r="D70" s="19"/>
+      <c r="A70" s="24"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="30"/>
       <c r="E70" s="9"/>
       <c r="F70" s="7"/>
-      <c r="G70" s="21"/>
-      <c r="H70" s="10"/>
-      <c r="I70" s="11"/>
+      <c r="G70" s="32"/>
+      <c r="H70" s="33"/>
+      <c r="I70" s="22"/>
     </row>
     <row r="71" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="19"/>
+      <c r="A71" s="24"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="30"/>
       <c r="E71" s="9"/>
       <c r="F71" s="7"/>
-      <c r="G71" s="21"/>
-      <c r="H71" s="10"/>
-      <c r="I71" s="11"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="33"/>
+      <c r="I71" s="22"/>
     </row>
     <row r="72" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="19"/>
+      <c r="A72" s="24"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="30"/>
       <c r="E72" s="9"/>
       <c r="F72" s="7"/>
-      <c r="G72" s="21"/>
-      <c r="H72" s="10"/>
-      <c r="I72" s="11"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="33"/>
+      <c r="I72" s="22"/>
     </row>
     <row r="73" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="16"/>
-      <c r="D73" s="19"/>
+      <c r="A73" s="24"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="27"/>
+      <c r="D73" s="30"/>
       <c r="E73" s="9"/>
       <c r="F73" s="7"/>
-      <c r="G73" s="21"/>
-      <c r="H73" s="10"/>
-      <c r="I73" s="11"/>
+      <c r="G73" s="32"/>
+      <c r="H73" s="33"/>
+      <c r="I73" s="22"/>
     </row>
     <row r="74" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="19"/>
+      <c r="A74" s="24"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="30"/>
       <c r="E74" s="9"/>
       <c r="F74" s="7"/>
-      <c r="G74" s="21"/>
-      <c r="H74" s="10"/>
-      <c r="I74" s="11"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="33"/>
+      <c r="I74" s="22"/>
     </row>
     <row r="75" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
-      <c r="D75" s="19"/>
+      <c r="A75" s="24"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="30"/>
       <c r="E75" s="9"/>
       <c r="F75" s="7"/>
-      <c r="G75" s="21"/>
-      <c r="H75" s="10"/>
-      <c r="I75" s="11"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="33"/>
+      <c r="I75" s="22"/>
     </row>
     <row r="76" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="16"/>
-      <c r="D76" s="19"/>
+      <c r="A76" s="24"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="30"/>
       <c r="E76" s="9"/>
       <c r="F76" s="7"/>
-      <c r="G76" s="21"/>
-      <c r="H76" s="10"/>
-      <c r="I76" s="11"/>
+      <c r="G76" s="32"/>
+      <c r="H76" s="33"/>
+      <c r="I76" s="22"/>
     </row>
     <row r="77" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="20"/>
+      <c r="A77" s="25"/>
+      <c r="B77" s="28"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="31"/>
       <c r="E77" s="8"/>
       <c r="F77" s="7"/>
-      <c r="G77" s="21"/>
-      <c r="H77" s="10"/>
-      <c r="I77" s="11"/>
+      <c r="G77" s="32"/>
+      <c r="H77" s="33"/>
+      <c r="I77" s="22"/>
     </row>
     <row r="78" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="12">
+      <c r="A78" s="23">
         <v>45100</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C78" s="15"/>
-      <c r="D78" s="18" t="s">
+      <c r="C78" s="26"/>
+      <c r="D78" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E78" s="9"/>
       <c r="F78" s="7"/>
-      <c r="G78" s="21" t="s">
+      <c r="G78" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H78" s="10" t="s">
+      <c r="H78" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="I78" s="11" t="s">
+      <c r="I78" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
-      <c r="D79" s="19"/>
+      <c r="A79" s="24"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="9"/>
       <c r="F79" s="7"/>
-      <c r="G79" s="21"/>
-      <c r="H79" s="10"/>
-      <c r="I79" s="11"/>
+      <c r="G79" s="32"/>
+      <c r="H79" s="33"/>
+      <c r="I79" s="22"/>
     </row>
     <row r="80" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A80" s="13"/>
-      <c r="B80" s="16"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="19"/>
+      <c r="A80" s="24"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="27"/>
+      <c r="D80" s="30"/>
       <c r="E80" s="9"/>
       <c r="F80" s="7"/>
-      <c r="G80" s="21"/>
-      <c r="H80" s="10"/>
-      <c r="I80" s="11"/>
+      <c r="G80" s="32"/>
+      <c r="H80" s="33"/>
+      <c r="I80" s="22"/>
     </row>
     <row r="81" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
-      <c r="B81" s="16"/>
-      <c r="C81" s="16"/>
-      <c r="D81" s="19"/>
+      <c r="A81" s="24"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="30"/>
       <c r="E81" s="9"/>
       <c r="F81" s="7"/>
-      <c r="G81" s="21"/>
-      <c r="H81" s="10"/>
-      <c r="I81" s="11"/>
+      <c r="G81" s="32"/>
+      <c r="H81" s="33"/>
+      <c r="I81" s="22"/>
     </row>
     <row r="82" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A82" s="13"/>
-      <c r="B82" s="16"/>
-      <c r="C82" s="16"/>
-      <c r="D82" s="19"/>
+      <c r="A82" s="24"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="30"/>
       <c r="E82" s="9"/>
       <c r="F82" s="7"/>
-      <c r="G82" s="21"/>
-      <c r="H82" s="10"/>
-      <c r="I82" s="11"/>
+      <c r="G82" s="32"/>
+      <c r="H82" s="33"/>
+      <c r="I82" s="22"/>
     </row>
     <row r="83" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
-      <c r="B83" s="16"/>
-      <c r="C83" s="16"/>
-      <c r="D83" s="19"/>
+      <c r="A83" s="24"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="27"/>
+      <c r="D83" s="30"/>
       <c r="E83" s="9"/>
       <c r="F83" s="7"/>
-      <c r="G83" s="21"/>
-      <c r="H83" s="10"/>
-      <c r="I83" s="11"/>
+      <c r="G83" s="32"/>
+      <c r="H83" s="33"/>
+      <c r="I83" s="22"/>
     </row>
     <row r="84" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
-      <c r="B84" s="16"/>
-      <c r="C84" s="16"/>
-      <c r="D84" s="19"/>
+      <c r="A84" s="24"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="30"/>
       <c r="E84" s="9"/>
       <c r="F84" s="7"/>
-      <c r="G84" s="21"/>
-      <c r="H84" s="10"/>
-      <c r="I84" s="11"/>
+      <c r="G84" s="32"/>
+      <c r="H84" s="33"/>
+      <c r="I84" s="22"/>
     </row>
     <row r="85" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A85" s="13"/>
-      <c r="B85" s="16"/>
-      <c r="C85" s="16"/>
-      <c r="D85" s="19"/>
+      <c r="A85" s="24"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="27"/>
+      <c r="D85" s="30"/>
       <c r="E85" s="9"/>
       <c r="F85" s="7"/>
-      <c r="G85" s="21"/>
-      <c r="H85" s="10"/>
-      <c r="I85" s="11"/>
+      <c r="G85" s="32"/>
+      <c r="H85" s="33"/>
+      <c r="I85" s="22"/>
     </row>
     <row r="86" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
-      <c r="B86" s="17"/>
-      <c r="C86" s="17"/>
-      <c r="D86" s="20"/>
+      <c r="A86" s="25"/>
+      <c r="B86" s="28"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="31"/>
       <c r="E86" s="8"/>
       <c r="F86" s="7"/>
-      <c r="G86" s="21"/>
-      <c r="H86" s="10"/>
-      <c r="I86" s="11"/>
+      <c r="G86" s="32"/>
+      <c r="H86" s="33"/>
+      <c r="I86" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="I6:I14"/>
-    <mergeCell ref="A6:A14"/>
-    <mergeCell ref="B6:B14"/>
-    <mergeCell ref="C6:C14"/>
-    <mergeCell ref="D6:D14"/>
-    <mergeCell ref="G6:G14"/>
-    <mergeCell ref="H6:H14"/>
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="A24:A32"/>
-    <mergeCell ref="A33:A41"/>
-    <mergeCell ref="A42:A50"/>
-    <mergeCell ref="B15:B23"/>
-    <mergeCell ref="B24:B32"/>
-    <mergeCell ref="B33:B41"/>
-    <mergeCell ref="B42:B50"/>
-    <mergeCell ref="C15:C23"/>
-    <mergeCell ref="D15:D23"/>
-    <mergeCell ref="G15:G23"/>
-    <mergeCell ref="H15:H23"/>
-    <mergeCell ref="I15:I23"/>
-    <mergeCell ref="C24:C32"/>
-    <mergeCell ref="D24:D32"/>
-    <mergeCell ref="G24:G32"/>
-    <mergeCell ref="H24:H32"/>
-    <mergeCell ref="I24:I32"/>
-    <mergeCell ref="C33:C41"/>
-    <mergeCell ref="D33:D41"/>
-    <mergeCell ref="G33:G41"/>
-    <mergeCell ref="H33:H41"/>
-    <mergeCell ref="I33:I41"/>
-    <mergeCell ref="C42:C50"/>
-    <mergeCell ref="D42:D50"/>
-    <mergeCell ref="G42:G50"/>
-    <mergeCell ref="H42:H50"/>
-    <mergeCell ref="I42:I50"/>
+    <mergeCell ref="H69:H77"/>
+    <mergeCell ref="I69:I77"/>
+    <mergeCell ref="A78:A86"/>
+    <mergeCell ref="B78:B86"/>
+    <mergeCell ref="C78:C86"/>
+    <mergeCell ref="D78:D86"/>
+    <mergeCell ref="G78:G86"/>
+    <mergeCell ref="H78:H86"/>
+    <mergeCell ref="I78:I86"/>
+    <mergeCell ref="A69:A77"/>
+    <mergeCell ref="B69:B77"/>
+    <mergeCell ref="C69:C77"/>
+    <mergeCell ref="D69:D77"/>
+    <mergeCell ref="G69:G77"/>
     <mergeCell ref="H51:H59"/>
     <mergeCell ref="I51:I59"/>
     <mergeCell ref="A60:A68"/>
@@ -2008,20 +2016,50 @@
     <mergeCell ref="C51:C59"/>
     <mergeCell ref="D51:D59"/>
     <mergeCell ref="G51:G59"/>
-    <mergeCell ref="H69:H77"/>
-    <mergeCell ref="I69:I77"/>
-    <mergeCell ref="A78:A86"/>
-    <mergeCell ref="B78:B86"/>
-    <mergeCell ref="C78:C86"/>
-    <mergeCell ref="D78:D86"/>
-    <mergeCell ref="G78:G86"/>
-    <mergeCell ref="H78:H86"/>
-    <mergeCell ref="I78:I86"/>
-    <mergeCell ref="A69:A77"/>
-    <mergeCell ref="B69:B77"/>
-    <mergeCell ref="C69:C77"/>
-    <mergeCell ref="D69:D77"/>
-    <mergeCell ref="G69:G77"/>
+    <mergeCell ref="C42:C50"/>
+    <mergeCell ref="D42:D50"/>
+    <mergeCell ref="G42:G50"/>
+    <mergeCell ref="H42:H50"/>
+    <mergeCell ref="I42:I50"/>
+    <mergeCell ref="C33:C41"/>
+    <mergeCell ref="D33:D41"/>
+    <mergeCell ref="G33:G41"/>
+    <mergeCell ref="H33:H41"/>
+    <mergeCell ref="I33:I41"/>
+    <mergeCell ref="C24:C32"/>
+    <mergeCell ref="D24:D32"/>
+    <mergeCell ref="G24:G32"/>
+    <mergeCell ref="H24:H32"/>
+    <mergeCell ref="I24:I32"/>
+    <mergeCell ref="C15:C23"/>
+    <mergeCell ref="D15:D23"/>
+    <mergeCell ref="G15:G23"/>
+    <mergeCell ref="H15:H23"/>
+    <mergeCell ref="I15:I23"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A24:A32"/>
+    <mergeCell ref="A33:A41"/>
+    <mergeCell ref="A42:A50"/>
+    <mergeCell ref="B15:B23"/>
+    <mergeCell ref="B24:B32"/>
+    <mergeCell ref="B33:B41"/>
+    <mergeCell ref="B42:B50"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="I6:I14"/>
+    <mergeCell ref="A6:A14"/>
+    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="C6:C14"/>
+    <mergeCell ref="D6:D14"/>
+    <mergeCell ref="G6:G14"/>
+    <mergeCell ref="H6:H14"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
@@ -2050,6 +2088,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010092E9E50D072E8F429600A5A4DFB79570" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="258385fc440d6e38a369b25097fe3065">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="09f4b8ca-d6aa-4fa0-a49f-053bce947579" xmlns:ns3="e0126794-098a-4121-936a-035bd9667ffd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca49e0bb93b4f43935efa4e0f1def3d0" ns2:_="" ns3:_="">
     <xsd:import namespace="09f4b8ca-d6aa-4fa0-a49f-053bce947579"/>
@@ -2266,16 +2313,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01E46630-91FC-4C92-932B-540B5F81C8D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4494570-4098-4156-98B4-69B9792AAFE3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2292,12 +2338,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01E46630-91FC-4C92-932B-540B5F81C8D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>